<commit_message>
Added CPS and BRFSS micro
</commit_message>
<xml_diff>
--- a/data-raw/microdata/microdata_variables.xlsx
+++ b/data-raw/microdata/microdata_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harri\OneDrive\GLP\glpdata\data-raw\microdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c93cd8282dd62d7/GLP/glpdata/data-raw/microdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="13_ncr:1_{87CBAAF1-9E57-4459-AE08-2F0DFE76093E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D42E4A97-B943-476B-ABFF-FC44EBD4E1AC}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{87CBAAF1-9E57-4459-AE08-2F0DFE76093E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3C11777D-C7C7-4C62-B974-9978FD4A4D1A}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
   <si>
     <t>Category</t>
   </si>
@@ -186,9 +186,6 @@
     <t>OWNCOST</t>
   </si>
   <si>
-    <t>burdened</t>
-  </si>
-  <si>
     <t>FTOTINC</t>
   </si>
   <si>
@@ -418,6 +415,12 @@
   </si>
   <si>
     <t>accidentally deleted</t>
+  </si>
+  <si>
+    <t>process data</t>
+  </si>
+  <si>
+    <t>cost_burden</t>
   </si>
 </sst>
 </file>
@@ -901,16 +904,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -926,6 +926,15 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1282,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1300,639 +1309,685 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="8"/>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="6"/>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="8"/>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+      <c r="E6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
-      <c r="E6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="8"/>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="8"/>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="8"/>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="8"/>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="8"/>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="8"/>
+      <c r="B18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="8"/>
+      <c r="B19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="8"/>
+      <c r="B20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="8"/>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="8"/>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="8"/>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="8"/>
+      <c r="B26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="8"/>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="8"/>
+      <c r="B28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="8"/>
+      <c r="B29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="8"/>
+      <c r="B30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5"/>
-      <c r="B17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="5"/>
-      <c r="B20" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="5"/>
-      <c r="B23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="5"/>
-      <c r="B26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="8"/>
+      <c r="B31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="8"/>
+      <c r="B32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="5"/>
-      <c r="B27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="5"/>
-      <c r="B28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="5"/>
-      <c r="B29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="5"/>
-      <c r="B30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-      <c r="E30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="5"/>
-      <c r="B31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="5"/>
-      <c r="B32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" t="s">
-        <v>106</v>
-      </c>
-    </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="5"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="5"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="3"/>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="5"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="3"/>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="5"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="3"/>
       <c r="E36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="4"/>
+      <c r="D37" s="3"/>
       <c r="E37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="8"/>
+      <c r="B38" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="5"/>
-      <c r="B38" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="8"/>
+      <c r="B39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="8"/>
+      <c r="B40" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="5"/>
-      <c r="B39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="8"/>
+      <c r="B41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="8"/>
+      <c r="B42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="8"/>
+      <c r="B43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="5"/>
-      <c r="B40" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="5"/>
-      <c r="B41" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="5"/>
-      <c r="B42" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="5"/>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="8"/>
+      <c r="B44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" t="s">
+      <c r="C44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="5"/>
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="8"/>
+      <c r="B45" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="4"/>
-      <c r="E44" t="s">
+      <c r="C45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="5"/>
-      <c r="B45" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="4"/>
-      <c r="E45" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="6"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>
-      <c r="B47" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" t="s">
-        <v>108</v>
-      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4"/>
-      <c r="B48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" t="s">
-        <v>109</v>
-      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4"/>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="6"/>
+      <c r="C52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="4"/>
-      <c r="D53" s="6"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="3"/>
+      <c r="D57" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C41:C42"/>
+  <mergeCells count="5">
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="A21:A24"/>
-    <mergeCell ref="C25:C27"/>
     <mergeCell ref="A37:A45"/>
-    <mergeCell ref="C43:C45"/>
     <mergeCell ref="A12:A20"/>
-    <mergeCell ref="C28:C36"/>
     <mergeCell ref="A25:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1962,7 +2017,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1970,7 +2025,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -1979,7 +2034,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -1988,19 +2043,19 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="3"/>
+      <c r="A5" s="9"/>
       <c r="B5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -2009,7 +2064,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="3"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -2018,19 +2073,19 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="3"/>
+      <c r="A9" s="9"/>
       <c r="B9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="3"/>
+      <c r="A10" s="9"/>
       <c r="B10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
@@ -2038,37 +2093,37 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="3"/>
+      <c r="A12" s="9"/>
       <c r="B12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="3"/>
+      <c r="A13" s="9"/>
       <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="3"/>
+      <c r="A14" s="9"/>
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="3"/>
+      <c r="A15" s="9"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="3"/>
+      <c r="A16" s="9"/>
       <c r="B16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
@@ -2076,7 +2131,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3"/>
+      <c r="A18" s="9"/>
       <c r="B18" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
microdata gets ~connected~ -add variables to excel
</commit_message>
<xml_diff>
--- a/data-raw/microdata/microdata_variables.xlsx
+++ b/data-raw/microdata/microdata_variables.xlsx
@@ -1,34 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c93cd8282dd62d7/GLP/glpdata/data-raw/microdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/mraisle_ad_unc_edu/Documents/glpdata/data-raw/microdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{87CBAAF1-9E57-4459-AE08-2F0DFE76093E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3C11777D-C7C7-4C62-B974-9978FD4A4D1A}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{87CBAAF1-9E57-4459-AE08-2F0DFE76093E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{ECDBD358-8156-8A4C-947F-882A2E08B3AA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="2080" windowWidth="20960" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACS" sheetId="1" r:id="rId1"/>
     <sheet name="CPS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="145">
   <si>
     <t>Category</t>
   </si>
@@ -421,13 +414,55 @@
   </si>
   <si>
     <t>cost_burden</t>
+  </si>
+  <si>
+    <t>CINETHH</t>
+  </si>
+  <si>
+    <t>digital divide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">access to internet </t>
+  </si>
+  <si>
+    <t>CILAPTOP</t>
+  </si>
+  <si>
+    <t>laptop, desktop, or notebook computer</t>
+  </si>
+  <si>
+    <t>CISMRTPHN</t>
+  </si>
+  <si>
+    <t>smartphone</t>
+  </si>
+  <si>
+    <t>CITABLET</t>
+  </si>
+  <si>
+    <t>tablet or other portable wireless computer</t>
+  </si>
+  <si>
+    <t>unsure if this overlaps with laptop</t>
+  </si>
+  <si>
+    <t>CIHISPEED</t>
+  </si>
+  <si>
+    <t>broadband (high speed) internet service such as cable, fiber optic, or DSL service</t>
+  </si>
+  <si>
+    <t>CIDIAL</t>
+  </si>
+  <si>
+    <t>dial-up service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -927,14 +962,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1291,24 +1326,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.05078125" style="2"/>
+    <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.3125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.20703125" customWidth="1"/>
-    <col min="5" max="5" width="44.1015625" customWidth="1"/>
-    <col min="7" max="7" width="17.20703125" customWidth="1"/>
-    <col min="8" max="8" width="36.3125" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1321,12 +1356,12 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1338,8 +1373,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:5" ht="32">
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>64</v>
       </c>
@@ -1353,8 +1388,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1364,8 +1399,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8"/>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1379,8 +1414,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8"/>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1390,8 +1425,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8"/>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
         <v>69</v>
       </c>
@@ -1403,8 +1438,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="8"/>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
         <v>75</v>
       </c>
@@ -1416,8 +1451,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8"/>
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="9"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1427,8 +1462,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1438,8 +1473,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8"/>
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1449,8 +1484,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:5" ht="16">
+      <c r="A12" s="9" t="s">
         <v>129</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1462,8 +1497,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8"/>
+    <row r="13" spans="1:5" ht="16">
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1475,8 +1510,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="8"/>
+    <row r="14" spans="1:5" ht="16">
+      <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1486,8 +1521,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:5" ht="16">
+      <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1497,8 +1532,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:5" ht="16">
+      <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1508,8 +1543,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1519,8 +1554,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="8"/>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>116</v>
       </c>
@@ -1531,8 +1566,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="8"/>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" s="9"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1541,8 +1576,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="8"/>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" s="9"/>
       <c r="B20" s="3" t="s">
         <v>117</v>
       </c>
@@ -1553,8 +1588,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:5" ht="16">
+      <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1568,8 +1603,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="8"/>
+    <row r="22" spans="1:5" ht="16">
+      <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1581,8 +1616,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="8"/>
+    <row r="23" spans="1:5" ht="16">
+      <c r="A23" s="9"/>
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
@@ -1594,8 +1629,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="8"/>
+    <row r="24" spans="1:5" ht="16">
+      <c r="A24" s="9"/>
       <c r="B24" s="3" t="s">
         <v>25</v>
       </c>
@@ -1607,8 +1642,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:5" ht="16">
+      <c r="A25" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1622,8 +1657,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="8"/>
+    <row r="26" spans="1:5" ht="16">
+      <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
@@ -1635,8 +1670,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="8"/>
+    <row r="27" spans="1:5" ht="16">
+      <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1648,8 +1683,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="8"/>
+    <row r="28" spans="1:5" ht="16">
+      <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>43</v>
       </c>
@@ -1661,8 +1696,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="8"/>
+    <row r="29" spans="1:5" ht="16">
+      <c r="A29" s="9"/>
       <c r="B29" s="3" t="s">
         <v>44</v>
       </c>
@@ -1674,8 +1709,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="8"/>
+    <row r="30" spans="1:5" ht="16">
+      <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
         <v>45</v>
       </c>
@@ -1687,8 +1722,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="8"/>
+    <row r="31" spans="1:5" ht="16">
+      <c r="A31" s="9"/>
       <c r="B31" s="3" t="s">
         <v>46</v>
       </c>
@@ -1700,8 +1735,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="8"/>
+    <row r="32" spans="1:5" ht="16">
+      <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
         <v>52</v>
       </c>
@@ -1713,8 +1748,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="8"/>
+    <row r="33" spans="1:5" ht="16">
+      <c r="A33" s="9"/>
       <c r="B33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1726,8 +1761,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="8"/>
+    <row r="34" spans="1:5" ht="16">
+      <c r="A34" s="9"/>
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
@@ -1739,8 +1774,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="8"/>
+    <row r="35" spans="1:5" ht="16">
+      <c r="A35" s="9"/>
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1752,8 +1787,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="8"/>
+    <row r="36" spans="1:5" ht="16">
+      <c r="A36" s="9"/>
       <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
@@ -1765,8 +1800,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:5" ht="16">
+      <c r="A37" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1780,8 +1815,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="8"/>
+    <row r="38" spans="1:5" ht="16">
+      <c r="A38" s="9"/>
       <c r="B38" s="3" t="s">
         <v>121</v>
       </c>
@@ -1793,8 +1828,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="8"/>
+    <row r="39" spans="1:5" ht="16">
+      <c r="A39" s="9"/>
       <c r="B39" s="3" t="s">
         <v>54</v>
       </c>
@@ -1806,8 +1841,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="8"/>
+    <row r="40" spans="1:5" ht="16">
+      <c r="A40" s="9"/>
       <c r="B40" s="3" t="s">
         <v>123</v>
       </c>
@@ -1819,8 +1854,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="8"/>
+    <row r="41" spans="1:5" ht="16">
+      <c r="A41" s="9"/>
       <c r="B41" s="3" t="s">
         <v>51</v>
       </c>
@@ -1832,8 +1867,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="8"/>
+    <row r="42" spans="1:5" ht="16">
+      <c r="A42" s="9"/>
       <c r="B42" s="3" t="s">
         <v>53</v>
       </c>
@@ -1845,8 +1880,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="8"/>
+    <row r="43" spans="1:5" ht="16">
+      <c r="A43" s="9"/>
       <c r="B43" s="3" t="s">
         <v>56</v>
       </c>
@@ -1858,8 +1893,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="8"/>
+    <row r="44" spans="1:5" ht="16">
+      <c r="A44" s="9"/>
       <c r="B44" s="3" t="s">
         <v>57</v>
       </c>
@@ -1871,8 +1906,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="8"/>
+    <row r="45" spans="1:5" ht="16">
+      <c r="A45" s="9"/>
       <c r="B45" s="3" t="s">
         <v>58</v>
       </c>
@@ -1884,103 +1919,159 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" ht="16">
       <c r="A46" s="4"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16">
       <c r="A47" s="4"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16">
       <c r="A48" s="4"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E48" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16">
       <c r="A49" s="4"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16">
       <c r="A50" s="3"/>
-      <c r="C50" s="3"/>
+      <c r="B50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="D50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E50" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16">
       <c r="A51" s="3"/>
-      <c r="B51" s="3" t="s">
-        <v>62</v>
+      <c r="B51" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>128</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D51" s="5"/>
       <c r="E51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="3"/>
-      <c r="B52" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E52" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C52" s="3"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" ht="16">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>128</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16">
       <c r="A54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>60</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" ht="16">
       <c r="A57" s="3"/>
-      <c r="D57" s="5"/>
+      <c r="B57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="3"/>
+      <c r="D59" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2003,9 +2094,9 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2016,16 +2107,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -2033,8 +2124,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:3">
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -2042,20 +2133,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:3">
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
+    <row r="6" spans="1:3">
+      <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -2063,8 +2154,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
+    <row r="8" spans="1:3">
+      <c r="A8" s="10"/>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -2072,71 +2163,71 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="9"/>
+    <row r="9" spans="1:3">
+      <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="9"/>
+    <row r="10" spans="1:3">
+      <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10"/>
       <c r="B12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="9"/>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10"/>
       <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:3">
+      <c r="A14" s="10"/>
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:3">
+      <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10"/>
       <c r="B18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2">
       <c r="A19" s="1"/>
     </row>
   </sheetData>

</xml_diff>